<commit_message>
forward sim plus particle filter for test data
</commit_message>
<xml_diff>
--- a/resources/data/test_data.xlsx
+++ b/resources/data/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\masters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\masters\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7D8B36F-D0FD-49DC-9ECC-0DA21B0BBF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CAFFD1A-CCE2-45D2-ACCC-79F03EB903E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="4095" windowWidth="38700" windowHeight="15435" xr2:uid="{28FDE054-CFB3-49EC-8405-3A0D0F540F7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{28FDE054-CFB3-49EC-8405-3A0D0F540F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="7">
   <si>
     <t>-</t>
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Symbol</t>
   </si>
 </sst>
 </file>
@@ -400,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40C480B-0F15-4C79-ADB5-15B231389B2D}">
-  <dimension ref="B2:F458"/>
+  <dimension ref="B1:F458"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,6 +426,23 @@
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>44488</v>
@@ -5700,7 +5732,7 @@
     </row>
     <row r="313" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B313" s="1">
-        <v>44478</v>
+        <v>44488</v>
       </c>
       <c r="C313" s="2">
         <v>0.73052083333333329</v>

</xml_diff>